<commit_message>
Actualización Escaleta_descripciones de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/Escaleta_LE_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/Escaleta_LE_08_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AULA PLANETA\PROCESO JUNIO 2015\GRADO OCTAVO\LE_08_01_CO\PROCESO Y CONTROL ESCALETAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -857,9 +857,6 @@
     <t>Banco de actividades: El anuncio publicitario</t>
   </si>
   <si>
-    <t>Actividad que propone la identificación de las características del periodo prehispánico o época precolombina</t>
-  </si>
-  <si>
     <t>Actividad para recordar las clases de oraciones y su estructura</t>
   </si>
   <si>
@@ -872,9 +869,6 @@
     <t xml:space="preserve">Actividad para interpretar anuncios publicitarios </t>
   </si>
   <si>
-    <t>Actividad diseñada para reconocer y comentar los elementos de un anuncio publicitario</t>
-  </si>
-  <si>
     <t>Interactivo para conocer los grupos indígenas de Colombia precolombina</t>
   </si>
   <si>
@@ -884,9 +878,6 @@
     <t>Actividad para repasar algunas características del periodo prehispánico</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para promover el conocimiento de un mito de la cultura precolombina </t>
-  </si>
-  <si>
     <t>Actividad para repasar las características de la literatura precolombina</t>
   </si>
   <si>
@@ -896,24 +887,12 @@
     <t>Actividad que promueve la comparación de las oraciones reflexivas y recíprocas</t>
   </si>
   <si>
-    <t>Actividad para afianzar los conocimientos sobre las oraciones reflexivas y recíprocas</t>
-  </si>
-  <si>
     <t>Actividad para practicar e identificar las palabras con diptongo</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para ejercitar la diferenciación de palabras a partir de la combinación de vocales </t>
-  </si>
-  <si>
     <t>Actividad que afianza la clasificación de palabras en diptongo triptongo e hiato</t>
   </si>
   <si>
-    <t>Actividad que permite identificar y jerarquizar la información partir de la intencionalidad</t>
-  </si>
-  <si>
-    <t>Interactivo para analizar un anuncio publicitario producido por los estudiantes</t>
-  </si>
-  <si>
     <t>Interactivo que aplica un proceso para producir un anuncio publicitario</t>
   </si>
   <si>
@@ -993,6 +972,27 @@
   </si>
   <si>
     <t>Interactivo para enfatizar en leyendas precolombinas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para conocer el periodo prehispánico de la época Precolombina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para comentar los elementos de un anuncio publicitario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para conocer y analizar un mito de la época precolombina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que profundiza en el tema de las oraciones reflexivas y recíprocas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para comparar el diptongo, el hiato y el triptongo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo para determinar las intenciones comunicativas de la publicidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo para analizar un anuncio publicitario </t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1310,10 +1310,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1603,8 +1607,8 @@
   <dimension ref="A1:U551"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,96 +1638,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="68" t="s">
+      <c r="Q1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="68" t="s">
+      <c r="U1" s="69" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="16" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="68"/>
-    </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="O2" s="69"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="69"/>
+    </row>
+    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="52" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>69</v>
@@ -1807,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>69</v>
@@ -1866,7 +1870,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>69</v>
@@ -1925,7 +1929,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="54" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>69</v>
@@ -1975,7 +1979,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="12"/>
       <c r="G7" s="53" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H7" s="6">
         <v>5</v>
@@ -1984,7 +1988,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>69</v>
@@ -2042,8 +2046,8 @@
       <c r="I8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="54" t="s">
-        <v>261</v>
+      <c r="J8" s="70" t="s">
+        <v>296</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>69</v>
@@ -2104,7 +2108,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>69</v>
@@ -2166,7 +2170,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="54" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>69</v>
@@ -2291,7 +2295,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="54" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>69</v>
@@ -2325,7 +2329,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>68</v>
       </c>
@@ -2353,8 +2357,8 @@
       <c r="I13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="54" t="s">
-        <v>265</v>
+      <c r="J13" s="70" t="s">
+        <v>297</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>69</v>
@@ -2408,7 +2412,7 @@
         <v>144</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="H14" s="6">
         <v>12</v>
@@ -2417,7 +2421,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>69</v>
@@ -2505,7 +2509,7 @@
         <v>169</v>
       </c>
       <c r="T15" s="65" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="U15" s="6" t="s">
         <v>171</v>
@@ -2538,7 +2542,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>69</v>
@@ -2590,7 +2594,7 @@
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="52" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="H17" s="6">
         <v>15</v>
@@ -2599,7 +2603,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="55" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>69</v>
@@ -2717,7 +2721,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="51" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>69</v>
@@ -2769,7 +2773,7 @@
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="52" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H20" s="6">
         <v>18</v>
@@ -2778,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="54" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>69</v>
@@ -2806,7 +2810,7 @@
         <v>169</v>
       </c>
       <c r="T20" s="67" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="U20" s="18" t="s">
         <v>171</v>
@@ -2867,7 +2871,7 @@
         <v>169</v>
       </c>
       <c r="T21" s="67" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="U21" s="18" t="s">
         <v>171</v>
@@ -2900,7 +2904,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="51" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>69</v>
@@ -2960,8 +2964,8 @@
       <c r="I23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="54" t="s">
-        <v>269</v>
+      <c r="J23" s="71" t="s">
+        <v>298</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>69</v>
@@ -3078,7 +3082,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="54" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>69</v>
@@ -3312,8 +3316,8 @@
       <c r="I29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="54" t="s">
-        <v>271</v>
+      <c r="J29" s="71" t="s">
+        <v>299</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>70</v>
@@ -3371,7 +3375,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="54" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>70</v>
@@ -3605,8 +3609,8 @@
       <c r="I34" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="32" t="s">
-        <v>273</v>
+      <c r="J34" s="71" t="s">
+        <v>300</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>69</v>
@@ -3633,7 +3637,7 @@
         <v>177</v>
       </c>
       <c r="T34" s="67" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="U34" s="18" t="s">
         <v>179</v>
@@ -3666,7 +3670,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>69</v>
@@ -3726,8 +3730,8 @@
       <c r="I36" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="31" t="s">
-        <v>274</v>
+      <c r="J36" s="71" t="s">
+        <v>301</v>
       </c>
       <c r="K36" s="6" t="s">
         <v>69</v>
@@ -3787,7 +3791,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>69</v>
@@ -3848,7 +3852,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="32" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>69</v>
@@ -3908,7 +3912,7 @@
         <v>19</v>
       </c>
       <c r="J39" s="32" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="K39" s="6" t="s">
         <v>69</v>
@@ -3996,7 +4000,7 @@
         <v>169</v>
       </c>
       <c r="T40" s="67" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="U40" s="18" t="s">
         <v>171</v>
@@ -4029,7 +4033,7 @@
         <v>20</v>
       </c>
       <c r="J41" s="32" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="K41" s="34" t="s">
         <v>69</v>
@@ -4057,7 +4061,7 @@
         <v>169</v>
       </c>
       <c r="T41" s="65" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U41" s="34" t="s">
         <v>171</v>
@@ -4088,7 +4092,7 @@
         <v>19</v>
       </c>
       <c r="J42" s="58" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="K42" s="60" t="s">
         <v>69</v>
@@ -4138,7 +4142,7 @@
       <c r="E43" s="45"/>
       <c r="F43" s="46"/>
       <c r="G43" s="52" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H43" s="6">
         <v>41</v>
@@ -4147,7 +4151,7 @@
         <v>20</v>
       </c>
       <c r="J43" s="56" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="K43" s="60" t="s">
         <v>69</v>
@@ -4160,7 +4164,7 @@
       </c>
       <c r="N43" s="16"/>
       <c r="O43" s="41" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="P43" s="60" t="s">
         <v>19</v>
@@ -4175,7 +4179,7 @@
         <v>169</v>
       </c>
       <c r="T43" s="67" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="U43" s="18" t="s">
         <v>171</v>
@@ -4265,7 +4269,7 @@
         <v>20</v>
       </c>
       <c r="J45" s="59" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="K45" s="62" t="s">
         <v>69</v>
@@ -4315,7 +4319,7 @@
       <c r="E46" s="41"/>
       <c r="F46" s="38"/>
       <c r="G46" s="52" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H46" s="6">
         <v>44</v>
@@ -4364,7 +4368,7 @@
         <v>20</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>69</v>
@@ -4421,7 +4425,7 @@
         <v>20</v>
       </c>
       <c r="J48" s="25" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="K48" s="38" t="s">
         <v>69</v>
@@ -13509,18 +13513,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
@@ -13529,6 +13521,18 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>